<commit_message>
update beforesuite keep extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/API_driven.xlsx
+++ b/src/test/resources/testdata/API_driven.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\github\GB-Demo\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CEDFF3-33DD-4DA8-A33A-442BD417EC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51674DD1-4865-4A8C-B689-8EC99A10F1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Content-Type</t>
   </si>
@@ -86,16 +86,31 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,10 +463,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,9 +503,52 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{CF9B27F1-8410-4B15-9B7C-FEE13A75AE3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{CF9B27F1-8410-4B15-9B7C-FEE13A75AE3C}">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -503,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3A6401-DB92-4553-BDAF-E68444DD7F60}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>

</xml_diff>